<commit_message>
Database and Excel readers with working tests
</commit_message>
<xml_diff>
--- a/ExcelReader/CS141roosterTest.xlsx
+++ b/ExcelReader/CS141roosterTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>YT</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>omalley_r@students.lynchbrg.edu</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -514,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +587,12 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2014</v>
+      </c>
+      <c r="B2">
+        <v>141</v>
+      </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
@@ -590,12 +602,18 @@
       <c r="E2" t="s">
         <v>16</v>
       </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
       <c r="G2">
         <v>359121</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
       </c>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
       <c r="J2" t="s">
         <v>23</v>
       </c>
@@ -611,8 +629,17 @@
       <c r="N2" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="O2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2014</v>
+      </c>
+      <c r="B3">
+        <v>141</v>
+      </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
@@ -622,26 +649,44 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
       <c r="G3">
         <v>359122</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
       </c>
+      <c r="I3" t="s">
+        <v>49</v>
+      </c>
       <c r="J3" t="s">
         <v>24</v>
       </c>
       <c r="K3" t="s">
         <v>25</v>
       </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
       <c r="M3" t="s">
         <v>38</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="O3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2014</v>
+      </c>
+      <c r="B4">
+        <v>141</v>
+      </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
@@ -651,26 +696,44 @@
       <c r="E4" t="s">
         <v>16</v>
       </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
       <c r="G4">
         <v>359123</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
       </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
       <c r="J4" t="s">
         <v>28</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
       </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
       <c r="M4" t="s">
         <v>39</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="O4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>141</v>
+      </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
@@ -680,26 +743,44 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
       <c r="G5">
         <v>359124</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
       </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
       <c r="J5" t="s">
         <v>30</v>
       </c>
       <c r="K5" t="s">
         <v>31</v>
       </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
       <c r="M5" t="s">
         <v>40</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="O5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>141</v>
+      </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
@@ -709,12 +790,18 @@
       <c r="E6" t="s">
         <v>16</v>
       </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
       <c r="G6">
         <v>359125</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
       </c>
+      <c r="I6" t="s">
+        <v>49</v>
+      </c>
       <c r="J6" t="s">
         <v>32</v>
       </c>
@@ -730,8 +817,17 @@
       <c r="N6" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="O6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2014</v>
+      </c>
+      <c r="B7">
+        <v>141</v>
+      </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
@@ -741,23 +837,35 @@
       <c r="E7" t="s">
         <v>16</v>
       </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
       <c r="G7">
         <v>359126</v>
       </c>
       <c r="H7" t="s">
         <v>18</v>
       </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
       <c r="J7" t="s">
         <v>35</v>
       </c>
       <c r="K7" t="s">
         <v>36</v>
       </c>
+      <c r="L7" t="s">
+        <v>36</v>
+      </c>
       <c r="M7" t="s">
         <v>42</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="O7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>